<commit_message>
Lab 7 changes made for linear regression. Added extra variables to multi-linear regression. Added region to merged data
</commit_message>
<xml_diff>
--- a/lab7/data/homelessness_data.xlsx
+++ b/lab7/data/homelessness_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidsosa/Code/school/regression-analysis/labs/lab7/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292384A6-0F22-6647-9A34-E1BD1325B42C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7262E1C-E551-744F-B091-9D44E8D7F0F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="13020" windowWidth="23840" windowHeight="8580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42820" yWindow="4540" windowWidth="23840" windowHeight="8580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Homelessness" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="948">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="947">
   <si>
     <t>Alabama</t>
   </si>
@@ -2830,9 +2830,6 @@
   </si>
   <si>
     <t>KY</t>
-  </si>
-  <si>
-    <t>state_name</t>
   </si>
   <si>
     <t>state_code</t>
@@ -3193,9 +3190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3206,13 +3201,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
         <v>934</v>
       </c>
-      <c r="B1" t="s">
-        <v>935</v>
-      </c>
       <c r="C1" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -3786,49 +3781,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBD448BA-3126-4967-99D6-3CA110BD445F}">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>934</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
         <v>52</v>
       </c>
       <c r="C1" t="s">
+        <v>935</v>
+      </c>
+      <c r="D1" t="s">
         <v>936</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>937</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>938</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>939</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>940</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>941</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>942</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>943</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>944</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>945</v>
-      </c>
-      <c r="M1" t="s">
-        <v>946</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>